<commit_message>
Pagina home e receita
</commit_message>
<xml_diff>
--- a/docs/Demonstrativo de Receitas Públicas e Privadas.xlsx
+++ b/docs/Demonstrativo de Receitas Públicas e Privadas.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anderson.eron\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camila.braga\Documents\GitHub\portal-transparencia-hci\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F3578AA-FF0F-4B07-9893-84FB6A14D5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF4E503-08B5-4044-ABF6-1AAF8143267B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{986F71AD-DD91-44FD-8681-3BBAE707547F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{986F71AD-DD91-44FD-8681-3BBAE707547F}"/>
   </bookViews>
   <sheets>
     <sheet name="Receitas Publicas x Privadas" sheetId="1" r:id="rId1"/>
+    <sheet name="Dados BI" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>DESCRIÇÃO</t>
   </si>
@@ -97,7 +98,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +136,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -159,7 +168,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -169,9 +178,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -179,9 +185,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -1012,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{832D77D0-B37D-4537-9643-A5CD9B40A026}">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,8 +1037,8 @@
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" hidden="1"/>
-    <col min="14" max="14" width="10.7109375" hidden="1"/>
+    <col min="13" max="13" width="12.7109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" hidden="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
@@ -1042,103 +1050,103 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>173598672</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>109475474</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>107404178</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <f>SUM(C5:C7)</f>
         <v>390478324</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="6">
+      <c r="C11" s="13">
         <v>2024</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="F11" s="6">
+      <c r="D11" s="13"/>
+      <c r="F11" s="13">
         <v>2023</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="I11" s="6">
+      <c r="G11" s="13"/>
+      <c r="I11" s="13">
         <v>2022</v>
       </c>
-      <c r="J11" s="6"/>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>21962882</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <f>+C12/$C$5</f>
         <v>0.12651526504764968</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>22980401</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <f>+F12/$C$6</f>
         <v>0.20991369263219631</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <v>19759098</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="8">
         <f>+I12/$C$7</f>
         <v>0.18396954725541495</v>
       </c>
@@ -1147,24 +1155,24 @@
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>6100052</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <f>+C13/$C$5</f>
         <v>3.5138817190951785E-2</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>3616363</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <f>+F13/$C$6</f>
         <v>3.3033545029455637E-2</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>3577398</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="8">
         <f>+I13/$C$7</f>
         <v>3.3307810428007747E-2</v>
       </c>
@@ -1173,24 +1181,24 @@
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>1471395</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <f>+C14/$C$5</f>
         <v>8.4758424880116597E-3</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <v>11999</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <f>+F14/$C$6</f>
         <v>1.0960445807249942E-4</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="7">
         <v>171594</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="8">
         <f>+I14/$C$7</f>
         <v>1.5976473466423253E-3</v>
       </c>
@@ -1199,61 +1207,61 @@
       <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>786319</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <f>+C15/$C$5</f>
         <v>4.5295219769883955E-3</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>774703</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <f>+F15/$C$6</f>
         <v>7.0764982483656567E-3</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="7">
         <v>2779408</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="8">
         <f>+I15/$C$7</f>
         <v>2.5878024968451412E-2</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <f>SUM(C12:C15)</f>
         <v>30320648</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="11">
         <f t="shared" ref="D16:J16" si="0">SUM(D12:D15)</f>
         <v>0.17465944670360151</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <f t="shared" si="0"/>
         <v>27383466</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="11">
         <f t="shared" si="0"/>
         <v>0.2501333403680901</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="10">
         <f t="shared" si="0"/>
         <v>26287498</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="11">
         <f t="shared" si="0"/>
         <v>0.24475302999851645</v>
       </c>
@@ -1262,24 +1270,24 @@
       <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>70485730</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <f>+C17/$C$5</f>
         <v>0.40602689633478301</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <v>43751197</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="8">
         <f>+F17/$C$6</f>
         <v>0.39964382341929844</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="7">
         <v>39368122</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="8">
         <f>+I17/$C$7</f>
         <v>0.3665418118092203</v>
       </c>
@@ -1288,61 +1296,61 @@
       <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>72792295</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <f>+C18/$C$5</f>
         <v>0.41931366272202819</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="7">
         <v>38126197</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <f>+F18/$C$6</f>
         <v>0.34826245191685584</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="7">
         <v>41406548</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="8">
         <f>+I18/$C$7</f>
         <v>0.38552083141495669</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="10">
         <f>SUM(C17:C18)</f>
         <v>143278025</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="11">
         <f t="shared" ref="D19:I19" si="1">SUM(D17:D18)</f>
         <v>0.82534055905681125</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="10">
         <f t="shared" si="1"/>
         <v>81877394</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="11">
         <f t="shared" si="1"/>
         <v>0.74790627533615428</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H19" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I19" s="10">
         <f t="shared" si="1"/>
         <v>80774670</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="11">
         <f>SUM(J17:J18)</f>
         <v>0.75206264322417704</v>
       </c>
@@ -1423,4 +1431,344 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1E03D9-5F5F-480C-9E5B-779E7E045AEC}">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="13">
+        <v>2024</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="E2" s="13">
+        <v>2023</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="H2" s="13">
+        <v>2022</v>
+      </c>
+      <c r="I2" s="13"/>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="7">
+        <v>173598672</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="7">
+        <v>21962882</v>
+      </c>
+      <c r="C3" s="8">
+        <f>+B3/$L$4</f>
+        <v>0.20448815315173308</v>
+      </c>
+      <c r="E3" s="7">
+        <v>22980401</v>
+      </c>
+      <c r="F3" s="8">
+        <f>+E3/$L$5</f>
+        <v>5.8851924902238617E-2</v>
+      </c>
+      <c r="H3" s="7">
+        <v>19759098</v>
+      </c>
+      <c r="I3" s="8">
+        <f>+H3/$L$4</f>
+        <v>0.18396954725541495</v>
+      </c>
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="7">
+        <v>109475474</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7">
+        <v>6100052</v>
+      </c>
+      <c r="C4" s="8">
+        <f>+B4/$L$4</f>
+        <v>5.6795295244473638E-2</v>
+      </c>
+      <c r="E4" s="7">
+        <v>3616363</v>
+      </c>
+      <c r="F4" s="8">
+        <f>+E4/$L$5</f>
+        <v>9.2613668358195473E-3</v>
+      </c>
+      <c r="H4" s="7">
+        <v>3577398</v>
+      </c>
+      <c r="I4" s="8">
+        <f t="shared" ref="I4:I6" si="0">+H4/$L$4</f>
+        <v>3.3307810428007747E-2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="7">
+        <v>107404178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1471395</v>
+      </c>
+      <c r="C5" s="8">
+        <f>+B5/$L$4</f>
+        <v>1.3699606732244624E-2</v>
+      </c>
+      <c r="E5" s="7">
+        <v>11999</v>
+      </c>
+      <c r="F5" s="8">
+        <f>+E5/$L$5</f>
+        <v>3.0728978441323163E-5</v>
+      </c>
+      <c r="H5" s="7">
+        <v>171594</v>
+      </c>
+      <c r="I5" s="8">
+        <f>+H5/$L$4</f>
+        <v>1.5976473466423253E-3</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="12">
+        <f>SUM(L2:L4)</f>
+        <v>390478324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7">
+        <v>786319</v>
+      </c>
+      <c r="C6" s="8">
+        <f>+B6/$L$4</f>
+        <v>7.3211211578752553E-3</v>
+      </c>
+      <c r="E6" s="7">
+        <v>774703</v>
+      </c>
+      <c r="F6" s="8">
+        <f>+E6/$L$5</f>
+        <v>1.9839846475063236E-3</v>
+      </c>
+      <c r="H6" s="7">
+        <v>2779408</v>
+      </c>
+      <c r="I6" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5878024968451412E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="10">
+        <f>SUM(B3:B6)</f>
+        <v>30320648</v>
+      </c>
+      <c r="C7" s="11">
+        <f t="shared" ref="C7:I7" si="1">SUM(C3:C6)</f>
+        <v>0.28230417628632659</v>
+      </c>
+      <c r="D7" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="1"/>
+        <v>27383466</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="1"/>
+        <v>7.0128005364005805E-2</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="1"/>
+        <v>26287498</v>
+      </c>
+      <c r="I7" s="11">
+        <f t="shared" si="1"/>
+        <v>0.24475302999851645</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7">
+        <v>70485730</v>
+      </c>
+      <c r="C8" s="8">
+        <f>+B8/$L$4</f>
+        <v>0.65626618361159095</v>
+      </c>
+      <c r="E8" s="7">
+        <v>43751197</v>
+      </c>
+      <c r="F8" s="8">
+        <f>+E8/$L$5</f>
+        <v>0.11204513621094113</v>
+      </c>
+      <c r="H8" s="7">
+        <v>39368122</v>
+      </c>
+      <c r="I8" s="8">
+        <f>+H8/$L$4</f>
+        <v>0.3665418118092203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7">
+        <v>72792295</v>
+      </c>
+      <c r="C9" s="8">
+        <f>+B9/$L$4</f>
+        <v>0.67774174483230998</v>
+      </c>
+      <c r="E9" s="7">
+        <v>38126197</v>
+      </c>
+      <c r="F9" s="8">
+        <f>+E9/$L$5</f>
+        <v>9.7639727115812966E-2</v>
+      </c>
+      <c r="H9" s="7">
+        <v>41406548</v>
+      </c>
+      <c r="I9" s="8">
+        <f>+H9/$L$4</f>
+        <v>0.38552083141495669</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="10">
+        <f>SUM(B8:B9)</f>
+        <v>143278025</v>
+      </c>
+      <c r="C10" s="11">
+        <f t="shared" ref="C10:H10" si="2">SUM(C8:C9)</f>
+        <v>1.334007928443901</v>
+      </c>
+      <c r="D10" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="10">
+        <f t="shared" si="2"/>
+        <v>81877394</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="2"/>
+        <v>0.2096848633267541</v>
+      </c>
+      <c r="G10" s="10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="2"/>
+        <v>80774670</v>
+      </c>
+      <c r="I10" s="11">
+        <f>SUM(I8:I9)</f>
+        <v>0.75206264322417704</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K14" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>